<commit_message>
Chau CHOSEN, Hola Select2 (modificado chosen style).
</commit_message>
<xml_diff>
--- a/documentos/Códigos Postales Argentina.xlsx
+++ b/documentos/Códigos Postales Argentina.xlsx
@@ -1,10 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="26731"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{319FAE76-D6A4-4CFA-9DD9-9713B14E7A1B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20400" windowHeight="7650"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -3171,7 +3172,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -3228,9 +3229,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema de Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2007 - 2010">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2007 - 2010">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -3268,9 +3269,9 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2007 - 2010">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -3305,7 +3306,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -3340,7 +3341,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2007 - 2010">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -3513,10 +3514,10 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:J2466"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A2451" workbookViewId="0">
       <selection sqref="A1:XFD1"/>
     </sheetView>
   </sheetViews>
@@ -3526,7 +3527,7 @@
     <col min="2" max="2" width="6.42578125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="1.5703125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="2.5703125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9.42578125" customWidth="1"/>
+    <col min="5" max="5" width="33.5703125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="2.5703125" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="1.5703125" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="3" bestFit="1" customWidth="1"/>
@@ -82705,7 +82706,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -82717,7 +82718,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>

</xml_diff>